<commit_message>
Analysis for zib HealthcareProvider
</commit_message>
<xml_diff>
--- a/maps/Location-and-Organization.xlsx
+++ b/maps/Location-and-Organization.xlsx
@@ -392,10 +392,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,12 +484,12 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -497,7 +497,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -505,7 +505,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -513,17 +513,17 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -538,27 +538,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-    </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
       <c r="B33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>